<commit_message>
KIBON-1591: Refacto + Anpassungen zwischenstand
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/Mahlzeitenverguenstigung.xlsx
+++ b/ebegu-server/src/main/resources/reporting/Mahlzeitenverguenstigung.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Kibon\Dev\kiBon\ebegu\ebegu-server\src\main\resources\reporting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DFA1302-4017-4BB9-8E38-70DD0E3DEFB2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B0B0419-C6F2-4BC7-8F74-AE3522AD2014}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="606" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="606" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="6" r:id="rId1"/>
@@ -41,9 +41,6 @@
     <t>{auswertungBis}</t>
   </si>
   <si>
-    <t>{auswertungPeriode}</t>
-  </si>
-  <si>
     <t>{bgNummer}</t>
   </si>
   <si>
@@ -83,9 +80,6 @@
     <t>{institutionTitle}</t>
   </si>
   <si>
-    <t>{periodeTitle}</t>
-  </si>
-  <si>
     <t>{parameterTitle}</t>
   </si>
   <si>
@@ -149,12 +143,6 @@
     <t>{kostenNebenmahlzeiten}</t>
   </si>
   <si>
-    <t>{verguenstigungProMahlzeitTitle}</t>
-  </si>
-  <si>
-    <t>{verguenstigungProMahlzeit}</t>
-  </si>
-  <si>
     <t>{berechneteMahlzeitenverguenstigungTitle}</t>
   </si>
   <si>
@@ -162,6 +150,18 @@
   </si>
   <si>
     <t>{mahlzeitenverguenstigungTitle}</t>
+  </si>
+  <si>
+    <t>{traegerschaftTitle}</t>
+  </si>
+  <si>
+    <t>{angebotTitle}</t>
+  </si>
+  <si>
+    <t>{traegerschaft}</t>
+  </si>
+  <si>
+    <t>{angebot}</t>
   </si>
 </sst>
 </file>
@@ -302,7 +302,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -316,13 +316,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -335,23 +328,24 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -761,254 +755,262 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:R11"/>
+  <dimension ref="A1:S10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q11" sqref="Q11"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="R16" sqref="R16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.6640625"/>
-    <col min="2" max="2" width="19.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.88671875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.88671875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.88671875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="27.109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="27.77734375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="27.33203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="28" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="30.44140625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="40" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="13.5546875" customWidth="1"/>
-    <col min="19" max="972" width="10.5546875"/>
+    <col min="1" max="1" width="20.7109375"/>
+    <col min="2" max="2" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="19.42578125" customWidth="1"/>
+    <col min="5" max="5" width="15.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="27.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="27.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="28" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="40" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.5703125" customWidth="1"/>
+    <col min="20" max="973" width="10.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="21" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:19" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B1" s="2"/>
-      <c r="C1" s="3"/>
+      <c r="C1" s="2"/>
       <c r="D1" s="2"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="2"/>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="C2"/>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="E2"/>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B3" s="4"/>
-      <c r="C3" s="5"/>
+      <c r="C3" s="4"/>
       <c r="D3" s="4"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="4"/>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C4"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4"/>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C5"/>
+      <c r="C5" s="20"/>
+      <c r="D5" s="20"/>
+      <c r="E5"/>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" s="7" t="s">
+    <row r="7" spans="1:19" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="D7" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="F7" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="G7" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="H7" s="18"/>
+      <c r="I7" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="J7" s="17"/>
+      <c r="K7" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="L7" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="M7" s="14"/>
+      <c r="N7" s="14"/>
+      <c r="O7" s="14"/>
+      <c r="P7" s="14"/>
+      <c r="Q7" s="14"/>
+      <c r="R7" s="14"/>
+    </row>
+    <row r="8" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="15"/>
+      <c r="B8" s="15"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="19"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="H8" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="I8" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="J8" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="K8" s="15"/>
+      <c r="L8" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="M8" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="N8" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="O8" s="14"/>
+      <c r="P8" s="14"/>
+      <c r="Q8" s="14"/>
+      <c r="R8" s="14"/>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A9" s="15"/>
+      <c r="B9" s="15"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="19"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="14"/>
+      <c r="I9" s="14"/>
+      <c r="J9" s="14"/>
+      <c r="K9" s="15"/>
+      <c r="L9" s="14"/>
+      <c r="M9" s="14"/>
+      <c r="N9" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="O9" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="P9" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q9" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="R9" s="7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A10" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="F10" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="H10" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="I10" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="J10" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="K10" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="8"/>
-      <c r="D6" s="9"/>
-    </row>
-    <row r="8" spans="1:18" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="C8" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="D8" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="E8" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="F8" s="19"/>
-      <c r="G8" s="18" t="s">
-        <v>24</v>
-      </c>
-      <c r="H8" s="20"/>
-      <c r="I8" s="17" t="s">
+      <c r="L10" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="M10" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="N10" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="J8" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="K8" s="22"/>
-      <c r="L8" s="22"/>
-      <c r="M8" s="22"/>
-      <c r="N8" s="22"/>
-      <c r="O8" s="22"/>
-      <c r="P8" s="22"/>
-      <c r="Q8" s="22"/>
-    </row>
-    <row r="9" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="17"/>
-      <c r="B9" s="17"/>
-      <c r="C9" s="21"/>
-      <c r="D9" s="17"/>
-      <c r="E9" s="22" t="s">
-        <v>20</v>
-      </c>
-      <c r="F9" s="22" t="s">
-        <v>21</v>
-      </c>
-      <c r="G9" s="22" t="s">
-        <v>20</v>
-      </c>
-      <c r="H9" s="22" t="s">
-        <v>21</v>
-      </c>
-      <c r="I9" s="17"/>
-      <c r="J9" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="K9" s="22" t="s">
-        <v>26</v>
-      </c>
-      <c r="L9" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="M9" s="22"/>
-      <c r="N9" s="22"/>
-      <c r="O9" s="22"/>
-      <c r="P9" s="22"/>
-      <c r="Q9" s="22"/>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A10" s="17"/>
-      <c r="B10" s="17"/>
-      <c r="C10" s="21"/>
-      <c r="D10" s="17"/>
-      <c r="E10" s="22"/>
-      <c r="F10" s="22"/>
-      <c r="G10" s="22"/>
-      <c r="H10" s="22"/>
-      <c r="I10" s="17"/>
-      <c r="J10" s="22"/>
-      <c r="K10" s="22"/>
-      <c r="L10" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="M10" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="N10" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="O10" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="P10" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="Q10" s="10" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A11" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="B11" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="D11" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="E11" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="F11" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="G11" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="H11" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="I11" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="J11" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="K11" s="14" t="s">
+      <c r="O10" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="P10" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q10" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="R10" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="S10" s="13" t="s">
         <v>13</v>
-      </c>
-      <c r="L11" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="M11" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="N11" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="O11" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="P11" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q11" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="R11" s="16" t="s">
-        <v>14</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="15">
-    <mergeCell ref="L9:Q9"/>
-    <mergeCell ref="J9:J10"/>
-    <mergeCell ref="K9:K10"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="I8:I10"/>
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="G9:G10"/>
-    <mergeCell ref="J8:Q8"/>
-    <mergeCell ref="H9:H10"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="A8:A10"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="C8:C10"/>
-    <mergeCell ref="D8:D10"/>
+  <mergeCells count="17">
+    <mergeCell ref="A7:A9"/>
+    <mergeCell ref="D7:D9"/>
+    <mergeCell ref="E7:E9"/>
+    <mergeCell ref="F7:F9"/>
+    <mergeCell ref="C7:C9"/>
+    <mergeCell ref="B7:B9"/>
+    <mergeCell ref="N8:R8"/>
+    <mergeCell ref="L8:L9"/>
+    <mergeCell ref="M8:M9"/>
+    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="G8:G9"/>
+    <mergeCell ref="K7:K9"/>
+    <mergeCell ref="I7:J7"/>
+    <mergeCell ref="I8:I9"/>
+    <mergeCell ref="L7:R7"/>
+    <mergeCell ref="J8:J9"/>
+    <mergeCell ref="G7:H7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
KIBON-1591: Query ok getrennt in zwei + falsche Klasse in der Converter + Statistik view Gemeinde Konfig pruefen + kleine Fix
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/Mahlzeitenverguenstigung.xlsx
+++ b/ebegu-server/src/main/resources/reporting/Mahlzeitenverguenstigung.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Kibon\Dev\kiBon\ebegu\ebegu-server\src\main\resources\reporting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B0B0419-C6F2-4BC7-8F74-AE3522AD2014}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F604F6D-EDF9-425F-AFA4-11C40D39D443}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="606" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="606" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="6" r:id="rId1"/>
@@ -325,13 +325,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -342,10 +345,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -757,34 +757,34 @@
   </sheetPr>
   <dimension ref="A1:S10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R16" sqref="R16"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="R10" sqref="R10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.7109375"/>
-    <col min="2" max="2" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="19.42578125" customWidth="1"/>
-    <col min="5" max="5" width="15.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="27.140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="27.7109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.6640625"/>
+    <col min="2" max="2" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="19.44140625" customWidth="1"/>
+    <col min="5" max="5" width="15.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.88671875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="27.109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="27.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="27.33203125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="28" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="40" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="13.5703125" customWidth="1"/>
-    <col min="20" max="973" width="10.5703125"/>
+    <col min="19" max="19" width="13.5546875" customWidth="1"/>
+    <col min="20" max="973" width="10.5546875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:19" ht="21" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
         <v>38</v>
       </c>
@@ -794,10 +794,10 @@
       <c r="E1" s="3"/>
       <c r="F1" s="2"/>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="E2"/>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>15</v>
       </c>
@@ -807,116 +807,116 @@
       <c r="E3" s="5"/>
       <c r="F3" s="4"/>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>16</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="20"/>
-      <c r="D4" s="20"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="13"/>
       <c r="E4"/>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>17</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="20"/>
-      <c r="D5" s="20"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="13"/>
       <c r="E5"/>
     </row>
-    <row r="7" spans="1:19" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="15" t="s">
+    <row r="7" spans="1:19" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="15" t="s">
+      <c r="B7" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="C7" s="15" t="s">
+      <c r="C7" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="D7" s="15" t="s">
+      <c r="D7" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="E7" s="19" t="s">
+      <c r="E7" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="F7" s="15" t="s">
+      <c r="F7" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="G7" s="16" t="s">
+      <c r="G7" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="H7" s="18"/>
-      <c r="I7" s="16" t="s">
+      <c r="H7" s="19"/>
+      <c r="I7" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="J7" s="17"/>
-      <c r="K7" s="15" t="s">
+      <c r="J7" s="18"/>
+      <c r="K7" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="L7" s="14" t="s">
+      <c r="L7" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="M7" s="14"/>
-      <c r="N7" s="14"/>
-      <c r="O7" s="14"/>
-      <c r="P7" s="14"/>
-      <c r="Q7" s="14"/>
-      <c r="R7" s="14"/>
+      <c r="M7" s="16"/>
+      <c r="N7" s="16"/>
+      <c r="O7" s="16"/>
+      <c r="P7" s="16"/>
+      <c r="Q7" s="16"/>
+      <c r="R7" s="16"/>
     </row>
-    <row r="8" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="15"/>
-      <c r="B8" s="15"/>
-      <c r="C8" s="15"/>
-      <c r="D8" s="15"/>
-      <c r="E8" s="19"/>
-      <c r="F8" s="15"/>
-      <c r="G8" s="14" t="s">
+    <row r="8" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="14"/>
+      <c r="B8" s="14"/>
+      <c r="C8" s="14"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="H8" s="14" t="s">
+      <c r="H8" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="I8" s="14" t="s">
+      <c r="I8" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="J8" s="14" t="s">
+      <c r="J8" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="K8" s="15"/>
-      <c r="L8" s="14" t="s">
+      <c r="K8" s="14"/>
+      <c r="L8" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="M8" s="14" t="s">
+      <c r="M8" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="N8" s="14" t="s">
+      <c r="N8" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="O8" s="14"/>
-      <c r="P8" s="14"/>
-      <c r="Q8" s="14"/>
-      <c r="R8" s="14"/>
+      <c r="O8" s="16"/>
+      <c r="P8" s="16"/>
+      <c r="Q8" s="16"/>
+      <c r="R8" s="16"/>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A9" s="15"/>
-      <c r="B9" s="15"/>
-      <c r="C9" s="15"/>
-      <c r="D9" s="15"/>
-      <c r="E9" s="19"/>
-      <c r="F9" s="15"/>
-      <c r="G9" s="14"/>
-      <c r="H9" s="14"/>
-      <c r="I9" s="14"/>
-      <c r="J9" s="14"/>
-      <c r="K9" s="15"/>
-      <c r="L9" s="14"/>
-      <c r="M9" s="14"/>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A9" s="14"/>
+      <c r="B9" s="14"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="16"/>
+      <c r="H9" s="16"/>
+      <c r="I9" s="16"/>
+      <c r="J9" s="16"/>
+      <c r="K9" s="14"/>
+      <c r="L9" s="16"/>
+      <c r="M9" s="16"/>
       <c r="N9" s="7" t="s">
         <v>28</v>
       </c>
@@ -933,7 +933,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A10" s="9" t="s">
         <v>3</v>
       </c>
@@ -973,33 +973,27 @@
       <c r="M10" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="N10" s="12" t="s">
+      <c r="N10" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="O10" s="12" t="s">
+      <c r="O10" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="P10" s="12" t="s">
+      <c r="P10" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="Q10" s="12" t="s">
+      <c r="Q10" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="R10" s="12" t="s">
+      <c r="R10" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="S10" s="13" t="s">
+      <c r="S10" s="12" t="s">
         <v>13</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="A7:A9"/>
-    <mergeCell ref="D7:D9"/>
-    <mergeCell ref="E7:E9"/>
-    <mergeCell ref="F7:F9"/>
-    <mergeCell ref="C7:C9"/>
-    <mergeCell ref="B7:B9"/>
     <mergeCell ref="N8:R8"/>
     <mergeCell ref="L8:L9"/>
     <mergeCell ref="M8:M9"/>
@@ -1011,6 +1005,12 @@
     <mergeCell ref="L7:R7"/>
     <mergeCell ref="J8:J9"/>
     <mergeCell ref="G7:H7"/>
+    <mergeCell ref="A7:A9"/>
+    <mergeCell ref="D7:D9"/>
+    <mergeCell ref="E7:E9"/>
+    <mergeCell ref="F7:F9"/>
+    <mergeCell ref="C7:C9"/>
+    <mergeCell ref="B7:B9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
KIBON-1771 add columns to datarow and excel
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/Mahlzeitenverguenstigung.xlsx
+++ b/ebegu-server/src/main/resources/reporting/Mahlzeitenverguenstigung.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Kibon\Dev\kiBon\ebegu\ebegu-server\src\main\resources\reporting\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\enja\IdeaProjects\ebegu\ebegu-server\src\main\resources\reporting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F604F6D-EDF9-425F-AFA4-11C40D39D443}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F310AD4-8801-477B-B705-4875B25A1A9C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="606" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23148" yWindow="1260" windowWidth="23256" windowHeight="12576" tabRatio="606" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="6" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="54">
   <si>
     <t>{auswertungVon}</t>
   </si>
@@ -162,14 +162,48 @@
   </si>
   <si>
     <t>{angebot}</t>
+  </si>
+  <si>
+    <t>{ibanTitle}</t>
+  </si>
+  <si>
+    <t>{iban}</t>
+  </si>
+  <si>
+    <t>{massgebendesEinkommenTitle}</t>
+  </si>
+  <si>
+    <t>{massgebendesEinkommenVorFamAbzugTitle}</t>
+  </si>
+  <si>
+    <t>{famGroesseTitle}</t>
+  </si>
+  <si>
+    <t>{massgebendesEinkommenNachFamAbzugTitle}</t>
+  </si>
+  <si>
+    <t>{massgebendesEinkommenVorFamAbzug}</t>
+  </si>
+  <si>
+    <t>{famGroesse}</t>
+  </si>
+  <si>
+    <t>{massgebendesEinkommenNachFamAbzug}</t>
+  </si>
+  <si>
+    <t>{sozialhilfebezuegerTitle}</t>
+  </si>
+  <si>
+    <t>{sozialhilfebezueger}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
+    <numFmt numFmtId="165" formatCode="&quot;CHF&quot;\ #,##0.00"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -216,7 +250,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -298,11 +332,35 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -327,25 +385,41 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -755,11 +829,9 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:S10"/>
+  <dimension ref="A1:X10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R10" sqref="R10"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -772,19 +844,20 @@
     <col min="8" max="8" width="13.88671875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15.109375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13.88671875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18.88671875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17.88671875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="27.109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="27.6640625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="27.33203125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="28" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="40" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="13.5546875" customWidth="1"/>
-    <col min="20" max="973" width="10.5546875"/>
+    <col min="11" max="15" width="13.88671875" customWidth="1"/>
+    <col min="16" max="16" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="18.88671875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="27.109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="27.6640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="28" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="40" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="13.5546875" customWidth="1"/>
+    <col min="25" max="978" width="10.5546875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="21" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:24" ht="21" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
         <v>38</v>
       </c>
@@ -794,10 +867,10 @@
       <c r="E1" s="3"/>
       <c r="F1" s="2"/>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
       <c r="E2"/>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>15</v>
       </c>
@@ -807,7 +880,7 @@
       <c r="E3" s="5"/>
       <c r="F3" s="4"/>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -818,7 +891,7 @@
       <c r="D4" s="13"/>
       <c r="E4"/>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -829,23 +902,23 @@
       <c r="D5" s="13"/>
       <c r="E5"/>
     </row>
-    <row r="7" spans="1:19" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="14" t="s">
+    <row r="7" spans="1:24" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="14" t="s">
+      <c r="B7" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="C7" s="14" t="s">
+      <c r="C7" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="D7" s="14" t="s">
+      <c r="D7" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="E7" s="15" t="s">
+      <c r="E7" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="F7" s="14" t="s">
+      <c r="F7" s="16" t="s">
         <v>20</v>
       </c>
       <c r="G7" s="17" t="s">
@@ -856,84 +929,111 @@
         <v>22</v>
       </c>
       <c r="J7" s="18"/>
-      <c r="K7" s="14" t="s">
+      <c r="K7" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="L7" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="M7" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="N7" s="15"/>
+      <c r="O7" s="15"/>
+      <c r="P7" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="L7" s="16" t="s">
+      <c r="Q7" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="M7" s="16"/>
-      <c r="N7" s="16"/>
-      <c r="O7" s="16"/>
-      <c r="P7" s="16"/>
-      <c r="Q7" s="16"/>
-      <c r="R7" s="16"/>
+      <c r="R7" s="15"/>
+      <c r="S7" s="15"/>
+      <c r="T7" s="15"/>
+      <c r="U7" s="15"/>
+      <c r="V7" s="15"/>
+      <c r="W7" s="15"/>
     </row>
-    <row r="8" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="14"/>
-      <c r="B8" s="14"/>
-      <c r="C8" s="14"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="15"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="16" t="s">
+    <row r="8" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="16"/>
+      <c r="B8" s="16"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="16"/>
+      <c r="E8" s="20"/>
+      <c r="F8" s="16"/>
+      <c r="G8" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="H8" s="16" t="s">
+      <c r="H8" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="I8" s="16" t="s">
+      <c r="I8" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="J8" s="16" t="s">
+      <c r="J8" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="K8" s="14"/>
-      <c r="L8" s="16" t="s">
+      <c r="K8" s="22"/>
+      <c r="L8" s="22"/>
+      <c r="M8" s="24" t="s">
+        <v>46</v>
+      </c>
+      <c r="N8" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="O8" s="24" t="s">
+        <v>48</v>
+      </c>
+      <c r="P8" s="16"/>
+      <c r="Q8" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="M8" s="16" t="s">
+      <c r="R8" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="N8" s="16" t="s">
+      <c r="S8" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="O8" s="16"/>
-      <c r="P8" s="16"/>
-      <c r="Q8" s="16"/>
-      <c r="R8" s="16"/>
+      <c r="T8" s="15"/>
+      <c r="U8" s="15"/>
+      <c r="V8" s="15"/>
+      <c r="W8" s="15"/>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A9" s="14"/>
-      <c r="B9" s="14"/>
-      <c r="C9" s="14"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="15"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="16"/>
-      <c r="H9" s="16"/>
-      <c r="I9" s="16"/>
-      <c r="J9" s="16"/>
-      <c r="K9" s="14"/>
-      <c r="L9" s="16"/>
-      <c r="M9" s="16"/>
-      <c r="N9" s="7" t="s">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A9" s="16"/>
+      <c r="B9" s="16"/>
+      <c r="C9" s="16"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="15"/>
+      <c r="I9" s="15"/>
+      <c r="J9" s="15"/>
+      <c r="K9" s="22"/>
+      <c r="L9" s="23"/>
+      <c r="M9" s="25"/>
+      <c r="N9" s="25"/>
+      <c r="O9" s="25"/>
+      <c r="P9" s="16"/>
+      <c r="Q9" s="15"/>
+      <c r="R9" s="15"/>
+      <c r="S9" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="O9" s="7" t="s">
+      <c r="T9" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="P9" s="7" t="s">
+      <c r="U9" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="Q9" s="7" t="s">
+      <c r="V9" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="R9" s="7" t="s">
+      <c r="W9" s="7" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A10" s="9" t="s">
         <v>3</v>
       </c>
@@ -964,53 +1064,74 @@
       <c r="J10" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="K10" s="11" t="s">
+      <c r="K10" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="L10" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="M10" s="26" t="s">
+        <v>49</v>
+      </c>
+      <c r="N10" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="O10" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="P10" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="L10" s="11" t="s">
+      <c r="Q10" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="M10" s="11" t="s">
+      <c r="R10" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="N10" s="20" t="s">
+      <c r="S10" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="O10" s="20" t="s">
+      <c r="T10" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="P10" s="20" t="s">
+      <c r="U10" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="Q10" s="20" t="s">
+      <c r="V10" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="R10" s="20" t="s">
+      <c r="W10" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="S10" s="12" t="s">
+      <c r="X10" s="12" t="s">
         <v>13</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="17">
-    <mergeCell ref="N8:R8"/>
-    <mergeCell ref="L8:L9"/>
-    <mergeCell ref="M8:M9"/>
-    <mergeCell ref="H8:H9"/>
-    <mergeCell ref="G8:G9"/>
+  <mergeCells count="23">
     <mergeCell ref="K7:K9"/>
-    <mergeCell ref="I7:J7"/>
-    <mergeCell ref="I8:I9"/>
-    <mergeCell ref="L7:R7"/>
-    <mergeCell ref="J8:J9"/>
-    <mergeCell ref="G7:H7"/>
     <mergeCell ref="A7:A9"/>
     <mergeCell ref="D7:D9"/>
     <mergeCell ref="E7:E9"/>
     <mergeCell ref="F7:F9"/>
     <mergeCell ref="C7:C9"/>
     <mergeCell ref="B7:B9"/>
+    <mergeCell ref="S8:W8"/>
+    <mergeCell ref="Q8:Q9"/>
+    <mergeCell ref="R8:R9"/>
+    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="G8:G9"/>
+    <mergeCell ref="P7:P9"/>
+    <mergeCell ref="I7:J7"/>
+    <mergeCell ref="I8:I9"/>
+    <mergeCell ref="Q7:W7"/>
+    <mergeCell ref="J8:J9"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="L7:L9"/>
+    <mergeCell ref="M7:O7"/>
+    <mergeCell ref="M8:M9"/>
+    <mergeCell ref="N8:N9"/>
+    <mergeCell ref="O8:O9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
KIBON-1771 add column headers
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/Mahlzeitenverguenstigung.xlsx
+++ b/ebegu-server/src/main/resources/reporting/Mahlzeitenverguenstigung.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\enja\IdeaProjects\ebegu\ebegu-server\src\main\resources\reporting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F310AD4-8801-477B-B705-4875B25A1A9C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E3E8E94-76C0-48AF-8EBD-81D991E23C5D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-23148" yWindow="1260" windowWidth="23256" windowHeight="12576" tabRatio="606" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -929,7 +929,7 @@
         <v>22</v>
       </c>
       <c r="J7" s="18"/>
-      <c r="K7" s="21" t="s">
+      <c r="K7" s="15" t="s">
         <v>52</v>
       </c>
       <c r="L7" s="21" t="s">
@@ -972,7 +972,7 @@
       <c r="J8" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="K8" s="22"/>
+      <c r="K8" s="15"/>
       <c r="L8" s="22"/>
       <c r="M8" s="24" t="s">
         <v>46</v>
@@ -1009,7 +1009,7 @@
       <c r="H9" s="15"/>
       <c r="I9" s="15"/>
       <c r="J9" s="15"/>
-      <c r="K9" s="22"/>
+      <c r="K9" s="15"/>
       <c r="L9" s="23"/>
       <c r="M9" s="25"/>
       <c r="N9" s="25"/>

</xml_diff>

<commit_message>
KIBON-1771 template style improvements
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/Mahlzeitenverguenstigung.xlsx
+++ b/ebegu-server/src/main/resources/reporting/Mahlzeitenverguenstigung.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\enja\IdeaProjects\ebegu\ebegu-server\src\main\resources\reporting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1F09533-E204-4E88-A5D9-71D07DEE42E3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDE84BB6-AA91-4AE2-9E7A-A5B969154740}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="1260" windowWidth="23256" windowHeight="12576" tabRatio="606" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="606" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="6" r:id="rId1"/>
@@ -360,7 +360,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -384,7 +384,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -393,32 +392,38 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -833,31 +838,32 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.6640625"/>
-    <col min="2" max="2" width="19.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="19.44140625" customWidth="1"/>
-    <col min="5" max="5" width="15.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.88671875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.88671875" bestFit="1" customWidth="1"/>
-    <col min="11" max="15" width="13.88671875" customWidth="1"/>
-    <col min="16" max="16" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="18.88671875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="17.88671875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="27.109375" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="27.6640625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.7109375"/>
+    <col min="2" max="2" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="19.42578125" customWidth="1"/>
+    <col min="5" max="5" width="15.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.85546875" style="26" customWidth="1"/>
+    <col min="12" max="15" width="13.85546875" customWidth="1"/>
+    <col min="16" max="16" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="27.140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="27.7109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="27.28515625" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="28" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="40" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="13.5546875" customWidth="1"/>
-    <col min="25" max="978" width="10.5546875"/>
+    <col min="24" max="24" width="13.5703125" customWidth="1"/>
+    <col min="25" max="978" width="10.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="21" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:24" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>38</v>
       </c>
@@ -867,10 +873,10 @@
       <c r="E1" s="3"/>
       <c r="F1" s="2"/>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="E2"/>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>15</v>
       </c>
@@ -880,143 +886,139 @@
       <c r="E3" s="5"/>
       <c r="F3" s="4"/>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>16</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
       <c r="E4"/>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>17</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="13"/>
-      <c r="D5" s="13"/>
       <c r="E5"/>
     </row>
-    <row r="7" spans="1:24" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="17" t="s">
+    <row r="7" spans="1:24" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="17" t="s">
+      <c r="B7" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="C7" s="17" t="s">
+      <c r="C7" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="D7" s="17" t="s">
+      <c r="D7" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="E7" s="18" t="s">
+      <c r="E7" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="F7" s="17" t="s">
+      <c r="F7" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="G7" s="19" t="s">
+      <c r="G7" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="H7" s="21"/>
-      <c r="I7" s="19" t="s">
+      <c r="H7" s="19"/>
+      <c r="I7" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="J7" s="20"/>
-      <c r="K7" s="17" t="s">
+      <c r="J7" s="18"/>
+      <c r="K7" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="L7" s="22" t="s">
+      <c r="L7" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="M7" s="16" t="s">
+      <c r="M7" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="N7" s="16"/>
-      <c r="O7" s="16"/>
-      <c r="P7" s="17" t="s">
+      <c r="N7" s="15"/>
+      <c r="O7" s="15"/>
+      <c r="P7" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="Q7" s="16" t="s">
+      <c r="Q7" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="R7" s="16"/>
-      <c r="S7" s="16"/>
-      <c r="T7" s="16"/>
-      <c r="U7" s="16"/>
-      <c r="V7" s="16"/>
-      <c r="W7" s="16"/>
+      <c r="R7" s="15"/>
+      <c r="S7" s="15"/>
+      <c r="T7" s="15"/>
+      <c r="U7" s="15"/>
+      <c r="V7" s="15"/>
+      <c r="W7" s="15"/>
     </row>
-    <row r="8" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="17"/>
-      <c r="B8" s="17"/>
-      <c r="C8" s="17"/>
-      <c r="D8" s="17"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="17"/>
-      <c r="G8" s="16" t="s">
+    <row r="8" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="16"/>
+      <c r="B8" s="16"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="16"/>
+      <c r="E8" s="25"/>
+      <c r="F8" s="16"/>
+      <c r="G8" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="H8" s="16" t="s">
+      <c r="H8" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="I8" s="16" t="s">
+      <c r="I8" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="J8" s="16" t="s">
+      <c r="J8" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="K8" s="17"/>
-      <c r="L8" s="23"/>
-      <c r="M8" s="25" t="s">
+      <c r="K8" s="16"/>
+      <c r="L8" s="21"/>
+      <c r="M8" s="23" t="s">
         <v>46</v>
       </c>
-      <c r="N8" s="25" t="s">
+      <c r="N8" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="O8" s="25" t="s">
+      <c r="O8" s="23" t="s">
         <v>48</v>
       </c>
-      <c r="P8" s="17"/>
-      <c r="Q8" s="16" t="s">
+      <c r="P8" s="16"/>
+      <c r="Q8" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="R8" s="16" t="s">
+      <c r="R8" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="S8" s="16" t="s">
+      <c r="S8" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="T8" s="16"/>
-      <c r="U8" s="16"/>
-      <c r="V8" s="16"/>
-      <c r="W8" s="16"/>
+      <c r="T8" s="15"/>
+      <c r="U8" s="15"/>
+      <c r="V8" s="15"/>
+      <c r="W8" s="15"/>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A9" s="17"/>
-      <c r="B9" s="17"/>
-      <c r="C9" s="17"/>
-      <c r="D9" s="17"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="17"/>
-      <c r="G9" s="16"/>
-      <c r="H9" s="16"/>
-      <c r="I9" s="16"/>
-      <c r="J9" s="16"/>
-      <c r="K9" s="17"/>
-      <c r="L9" s="24"/>
-      <c r="M9" s="26"/>
-      <c r="N9" s="26"/>
-      <c r="O9" s="26"/>
-      <c r="P9" s="17"/>
-      <c r="Q9" s="16"/>
-      <c r="R9" s="16"/>
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A9" s="16"/>
+      <c r="B9" s="16"/>
+      <c r="C9" s="16"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="25"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="15"/>
+      <c r="I9" s="15"/>
+      <c r="J9" s="15"/>
+      <c r="K9" s="16"/>
+      <c r="L9" s="22"/>
+      <c r="M9" s="24"/>
+      <c r="N9" s="24"/>
+      <c r="O9" s="24"/>
+      <c r="P9" s="16"/>
+      <c r="Q9" s="15"/>
+      <c r="R9" s="15"/>
       <c r="S9" s="7" t="s">
         <v>28</v>
       </c>
@@ -1033,7 +1035,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
         <v>3</v>
       </c>
@@ -1064,19 +1066,19 @@
       <c r="J10" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="K10" s="9" t="s">
+      <c r="K10" s="27" t="s">
         <v>53</v>
       </c>
       <c r="L10" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="M10" s="15" t="s">
+      <c r="M10" s="14" t="s">
         <v>49</v>
       </c>
       <c r="N10" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="O10" s="15" t="s">
+      <c r="O10" s="14" t="s">
         <v>51</v>
       </c>
       <c r="P10" s="11" t="s">
@@ -1088,19 +1090,19 @@
       <c r="R10" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="S10" s="14" t="s">
+      <c r="S10" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="T10" s="14" t="s">
+      <c r="T10" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="U10" s="14" t="s">
+      <c r="U10" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="V10" s="14" t="s">
+      <c r="V10" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="W10" s="14" t="s">
+      <c r="W10" s="13" t="s">
         <v>37</v>
       </c>
       <c r="X10" s="12" t="s">
@@ -1109,6 +1111,13 @@
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="K7:K9"/>
+    <mergeCell ref="A7:A9"/>
+    <mergeCell ref="D7:D9"/>
+    <mergeCell ref="E7:E9"/>
+    <mergeCell ref="F7:F9"/>
+    <mergeCell ref="C7:C9"/>
+    <mergeCell ref="B7:B9"/>
     <mergeCell ref="S8:W8"/>
     <mergeCell ref="Q8:Q9"/>
     <mergeCell ref="R8:R9"/>
@@ -1125,13 +1134,6 @@
     <mergeCell ref="M8:M9"/>
     <mergeCell ref="N8:N9"/>
     <mergeCell ref="O8:O9"/>
-    <mergeCell ref="K7:K9"/>
-    <mergeCell ref="A7:A9"/>
-    <mergeCell ref="D7:D9"/>
-    <mergeCell ref="E7:E9"/>
-    <mergeCell ref="F7:F9"/>
-    <mergeCell ref="C7:C9"/>
-    <mergeCell ref="B7:B9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
KIBON-2166: add fallnummer to Mahlzeitenverguenstigung statistik
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/Mahlzeitenverguenstigung.xlsx
+++ b/ebegu-server/src/main/resources/reporting/Mahlzeitenverguenstigung.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\enja\IdeaProjects\ebegu\ebegu-server\src\main\resources\reporting\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\new\ebegu\ebegu-server\src\main\resources\reporting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDE84BB6-AA91-4AE2-9E7A-A5B969154740}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F004BD9F-C241-4C50-BFF8-A03284A2CB6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="606" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="606" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="6" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="56">
   <si>
     <t>{auswertungVon}</t>
   </si>
@@ -195,6 +195,12 @@
   </si>
   <si>
     <t>{sozialhilfebezueger}</t>
+  </si>
+  <si>
+    <t>{fallNummer}</t>
+  </si>
+  <si>
+    <t>{fallNummerTitle}</t>
   </si>
 </sst>
 </file>
@@ -360,7 +366,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -386,12 +392,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -416,15 +431,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -834,9 +841,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:X10"/>
+  <dimension ref="A1:Y10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P10" sqref="P10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -849,21 +858,21 @@
     <col min="8" max="8" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.85546875" style="26" customWidth="1"/>
-    <col min="12" max="15" width="13.85546875" customWidth="1"/>
-    <col min="16" max="16" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="27.140625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="27.7109375" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="27.28515625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="28" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="40" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="13.5703125" customWidth="1"/>
-    <col min="25" max="978" width="10.5703125"/>
+    <col min="11" max="11" width="13.85546875" style="15" customWidth="1"/>
+    <col min="12" max="16" width="13.85546875" customWidth="1"/>
+    <col min="17" max="17" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="27.140625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="27.7109375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="28" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="40" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="13.5703125" customWidth="1"/>
+    <col min="26" max="979" width="10.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:25" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>38</v>
       </c>
@@ -873,10 +882,10 @@
       <c r="E1" s="3"/>
       <c r="F1" s="2"/>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="E2"/>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>15</v>
       </c>
@@ -886,7 +895,7 @@
       <c r="E3" s="5"/>
       <c r="F3" s="4"/>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -895,7 +904,7 @@
       </c>
       <c r="E4"/>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -904,138 +913,143 @@
       </c>
       <c r="E5"/>
     </row>
-    <row r="7" spans="1:24" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="16" t="s">
+    <row r="7" spans="1:25" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="16" t="s">
+      <c r="B7" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="C7" s="16" t="s">
+      <c r="C7" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="D7" s="16" t="s">
+      <c r="D7" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="E7" s="25" t="s">
+      <c r="E7" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="F7" s="16" t="s">
+      <c r="F7" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="G7" s="17" t="s">
+      <c r="G7" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="H7" s="19"/>
-      <c r="I7" s="17" t="s">
+      <c r="H7" s="22"/>
+      <c r="I7" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="J7" s="18"/>
-      <c r="K7" s="16" t="s">
+      <c r="J7" s="21"/>
+      <c r="K7" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="L7" s="20" t="s">
+      <c r="L7" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="M7" s="15" t="s">
+      <c r="M7" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="N7" s="15"/>
-      <c r="O7" s="15"/>
-      <c r="P7" s="16" t="s">
+      <c r="N7" s="19"/>
+      <c r="O7" s="19"/>
+      <c r="P7" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q7" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="Q7" s="15" t="s">
+      <c r="R7" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="R7" s="15"/>
-      <c r="S7" s="15"/>
-      <c r="T7" s="15"/>
-      <c r="U7" s="15"/>
-      <c r="V7" s="15"/>
-      <c r="W7" s="15"/>
+      <c r="S7" s="19"/>
+      <c r="T7" s="19"/>
+      <c r="U7" s="19"/>
+      <c r="V7" s="19"/>
+      <c r="W7" s="19"/>
+      <c r="X7" s="19"/>
     </row>
-    <row r="8" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="16"/>
-      <c r="B8" s="16"/>
-      <c r="C8" s="16"/>
-      <c r="D8" s="16"/>
-      <c r="E8" s="25"/>
-      <c r="F8" s="16"/>
-      <c r="G8" s="15" t="s">
+    <row r="8" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="17"/>
+      <c r="B8" s="17"/>
+      <c r="C8" s="17"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="17"/>
+      <c r="G8" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="H8" s="15" t="s">
+      <c r="H8" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="I8" s="15" t="s">
+      <c r="I8" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="J8" s="15" t="s">
+      <c r="J8" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="K8" s="16"/>
-      <c r="L8" s="21"/>
-      <c r="M8" s="23" t="s">
+      <c r="K8" s="17"/>
+      <c r="L8" s="24"/>
+      <c r="M8" s="26" t="s">
         <v>46</v>
       </c>
-      <c r="N8" s="23" t="s">
+      <c r="N8" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="O8" s="23" t="s">
+      <c r="O8" s="26" t="s">
         <v>48</v>
       </c>
-      <c r="P8" s="16"/>
-      <c r="Q8" s="15" t="s">
+      <c r="P8" s="17"/>
+      <c r="Q8" s="17"/>
+      <c r="R8" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="R8" s="15" t="s">
+      <c r="S8" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="S8" s="15" t="s">
+      <c r="T8" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="T8" s="15"/>
-      <c r="U8" s="15"/>
-      <c r="V8" s="15"/>
-      <c r="W8" s="15"/>
+      <c r="U8" s="19"/>
+      <c r="V8" s="19"/>
+      <c r="W8" s="19"/>
+      <c r="X8" s="19"/>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A9" s="16"/>
-      <c r="B9" s="16"/>
-      <c r="C9" s="16"/>
-      <c r="D9" s="16"/>
-      <c r="E9" s="25"/>
-      <c r="F9" s="16"/>
-      <c r="G9" s="15"/>
-      <c r="H9" s="15"/>
-      <c r="I9" s="15"/>
-      <c r="J9" s="15"/>
-      <c r="K9" s="16"/>
-      <c r="L9" s="22"/>
-      <c r="M9" s="24"/>
-      <c r="N9" s="24"/>
-      <c r="O9" s="24"/>
-      <c r="P9" s="16"/>
-      <c r="Q9" s="15"/>
-      <c r="R9" s="15"/>
-      <c r="S9" s="7" t="s">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A9" s="17"/>
+      <c r="B9" s="17"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="17"/>
+      <c r="G9" s="19"/>
+      <c r="H9" s="19"/>
+      <c r="I9" s="19"/>
+      <c r="J9" s="19"/>
+      <c r="K9" s="17"/>
+      <c r="L9" s="25"/>
+      <c r="M9" s="27"/>
+      <c r="N9" s="27"/>
+      <c r="O9" s="27"/>
+      <c r="P9" s="17"/>
+      <c r="Q9" s="17"/>
+      <c r="R9" s="19"/>
+      <c r="S9" s="19"/>
+      <c r="T9" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="T9" s="7" t="s">
+      <c r="U9" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="U9" s="7" t="s">
+      <c r="V9" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="V9" s="7" t="s">
+      <c r="W9" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="W9" s="7" t="s">
+      <c r="X9" s="7" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
         <v>3</v>
       </c>
@@ -1066,7 +1080,7 @@
       <c r="J10" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="K10" s="27" t="s">
+      <c r="K10" s="16" t="s">
         <v>53</v>
       </c>
       <c r="L10" s="9" t="s">
@@ -1081,52 +1095,46 @@
       <c r="O10" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="P10" s="11" t="s">
+      <c r="P10" s="28" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q10" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="Q10" s="11" t="s">
+      <c r="R10" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="R10" s="11" t="s">
+      <c r="S10" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="S10" s="13" t="s">
+      <c r="T10" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="T10" s="13" t="s">
+      <c r="U10" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="U10" s="13" t="s">
+      <c r="V10" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="V10" s="13" t="s">
+      <c r="W10" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="W10" s="13" t="s">
+      <c r="X10" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="X10" s="12" t="s">
+      <c r="Y10" s="12" t="s">
         <v>13</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="23">
-    <mergeCell ref="K7:K9"/>
-    <mergeCell ref="A7:A9"/>
-    <mergeCell ref="D7:D9"/>
-    <mergeCell ref="E7:E9"/>
-    <mergeCell ref="F7:F9"/>
-    <mergeCell ref="C7:C9"/>
-    <mergeCell ref="B7:B9"/>
-    <mergeCell ref="S8:W8"/>
-    <mergeCell ref="Q8:Q9"/>
-    <mergeCell ref="R8:R9"/>
+  <mergeCells count="24">
+    <mergeCell ref="S8:S9"/>
     <mergeCell ref="H8:H9"/>
     <mergeCell ref="G8:G9"/>
-    <mergeCell ref="P7:P9"/>
+    <mergeCell ref="Q7:Q9"/>
     <mergeCell ref="I7:J7"/>
     <mergeCell ref="I8:I9"/>
-    <mergeCell ref="Q7:W7"/>
+    <mergeCell ref="R7:X7"/>
     <mergeCell ref="J8:J9"/>
     <mergeCell ref="G7:H7"/>
     <mergeCell ref="L7:L9"/>
@@ -1134,6 +1142,16 @@
     <mergeCell ref="M8:M9"/>
     <mergeCell ref="N8:N9"/>
     <mergeCell ref="O8:O9"/>
+    <mergeCell ref="K7:K9"/>
+    <mergeCell ref="P7:P9"/>
+    <mergeCell ref="T8:X8"/>
+    <mergeCell ref="R8:R9"/>
+    <mergeCell ref="A7:A9"/>
+    <mergeCell ref="D7:D9"/>
+    <mergeCell ref="E7:E9"/>
+    <mergeCell ref="F7:F9"/>
+    <mergeCell ref="C7:C9"/>
+    <mergeCell ref="B7:B9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId1"/>

</xml_diff>